<commit_message>
Modified test data for integration test
</commit_message>
<xml_diff>
--- a/integration/10x.xlsx
+++ b/integration/10x.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/ait/repos/ingest-integration-tests/tests/fixtures/datasets/10x/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/ait/repos/ingest-archiver/integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF14E6C-90AB-CC4F-B4B1-2AC89F3F6CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4955F8EA-F6E6-6941-A493-785BB8D22F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="696">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -1647,12 +1647,6 @@
     <t>cell_ID_1</t>
   </si>
   <si>
-    <t>This is a dummy cell</t>
-  </si>
-  <si>
-    <t>This is a dummy donor cell</t>
-  </si>
-  <si>
     <t>specimen_ID_1</t>
   </si>
   <si>
@@ -1998,9 +1992,6 @@
     <t>10x fastq files</t>
   </si>
   <si>
-    <t>WSSS_THYst9384954_S1_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
     <t>10x_5_v1</t>
   </si>
   <si>
@@ -2010,12 +2001,6 @@
     <t>lib_15</t>
   </si>
   <si>
-    <t>WSSS_THYst9384954_S1_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>WSSS_THYst9384955_S1_L001_I1_001.fastq.gz</t>
-  </si>
-  <si>
     <t>index1</t>
   </si>
   <si>
@@ -2107,6 +2092,42 @@
   </si>
   <si>
     <t>This is a test dataset for ENA 10x files submission. The description must be 50 characters or above.</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_R1_002.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_R2_002.fastq.gz</t>
+  </si>
+  <si>
+    <t>cell_ID_2</t>
+  </si>
+  <si>
+    <t>This is a dummy donor cell 1</t>
+  </si>
+  <si>
+    <t>This is a dummy donor cell 2</t>
+  </si>
+  <si>
+    <t>This is a dummy cell 1</t>
+  </si>
+  <si>
+    <t>This is a dummy cell 2</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L001_I1_002.fastq.gz</t>
+  </si>
+  <si>
+    <t>process.process_core.process_id</t>
   </si>
 </sst>
 </file>
@@ -2528,7 +2549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2605,7 +2626,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2614,7 +2635,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2631,16 +2652,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2657,13 +2678,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B6" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="C6" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -2794,13 +2815,13 @@
         <v>411</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>604</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2818,31 +2839,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C6" t="s">
+        <v>557</v>
+      </c>
+      <c r="D6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" t="s">
+        <v>552</v>
+      </c>
+      <c r="F6" t="s">
+        <v>553</v>
+      </c>
+      <c r="G6" t="s">
+        <v>560</v>
+      </c>
+      <c r="H6" t="s">
         <v>558</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>559</v>
-      </c>
-      <c r="D6" t="s">
-        <v>553</v>
-      </c>
-      <c r="E6" t="s">
-        <v>554</v>
-      </c>
-      <c r="F6" t="s">
-        <v>555</v>
-      </c>
-      <c r="G6" t="s">
-        <v>562</v>
-      </c>
-      <c r="H6" t="s">
-        <v>560</v>
-      </c>
-      <c r="I6" t="s">
-        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -3001,22 +3022,22 @@
         <v>420</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>623</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>625</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>427</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3037,34 +3058,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>562</v>
+      </c>
+      <c r="B6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C6" t="s">
         <v>564</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" t="s">
+        <v>552</v>
+      </c>
+      <c r="F6" t="s">
+        <v>553</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="J6" t="s">
         <v>565</v>
-      </c>
-      <c r="C6" t="s">
-        <v>566</v>
-      </c>
-      <c r="D6" t="s">
-        <v>553</v>
-      </c>
-      <c r="E6" t="s">
-        <v>554</v>
-      </c>
-      <c r="F6" t="s">
-        <v>555</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="J6" t="s">
-        <v>567</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3243,13 +3264,13 @@
         <v>443</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>445</v>
@@ -3261,31 +3282,31 @@
         <v>447</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>671</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>676</v>
       </c>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
@@ -3341,46 +3362,46 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>573</v>
-      </c>
       <c r="K6" s="7" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -3393,20 +3414,20 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>573</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="AE6" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AF6" s="3" t="s">
         <v>576</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="16" x14ac:dyDescent="0.2">
@@ -3619,25 +3640,25 @@
         <v>468</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>609</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3664,38 +3685,38 @@
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
         <v>487</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -3820,7 +3841,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -3844,7 +3865,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -4005,7 +4026,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4014,7 +4035,7 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4105,7 +4126,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4601,10 +4622,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -4831,13 +4852,13 @@
         <v>512</v>
       </c>
       <c r="Y6" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="Z6" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AA6" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="AB6">
         <v>22</v>
@@ -5254,10 +5275,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5278,13 +5299,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>596</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>598</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5302,7 +5323,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5314,7 +5335,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5390,7 +5411,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>522</v>
@@ -5426,22 +5447,22 @@
         <v>524</v>
       </c>
       <c r="O6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="P6" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="Q6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="U6" t="s">
         <v>526</v>
@@ -5468,7 +5489,7 @@
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AD6">
         <v>5</v>
@@ -5492,7 +5513,7 @@
         <v>498</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -5502,10 +5523,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5600,13 +5621,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -5795,10 +5816,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -5837,25 +5858,25 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>630</v>
-      </c>
       <c r="X4" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
@@ -5906,10 +5927,10 @@
         <v>534</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>535</v>
+        <v>691</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>536</v>
+        <v>689</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -5921,28 +5942,28 @@
         <v>502</v>
       </c>
       <c r="I6" t="s">
+        <v>536</v>
+      </c>
+      <c r="J6" t="s">
+        <v>537</v>
+      </c>
+      <c r="K6" t="s">
         <v>538</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>539</v>
       </c>
-      <c r="K6" t="s">
-        <v>540</v>
-      </c>
-      <c r="L6" t="s">
-        <v>541</v>
-      </c>
       <c r="M6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="P6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="Q6">
         <v>10</v>
@@ -5957,13 +5978,13 @@
         <v>506</v>
       </c>
       <c r="U6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="V6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="W6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -5972,19 +5993,105 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AA6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AB6" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="D7" s="3">
+        <v>9606</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="AC6" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>564</v>
+      <c r="K7" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="N7" s="3">
+        <v>98.7</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>10</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>2217</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -5994,10 +6101,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6006,18 +6113,19 @@
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="9" width="25.6640625" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="45.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="45.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>355</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>357</v>
@@ -6041,19 +6149,20 @@
         <v>378</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>356</v>
       </c>
@@ -6079,16 +6188,17 @@
         <v>379</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -6114,30 +6224,31 @@
         <v>380</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>641</v>
-      </c>
+        <v>638</v>
+      </c>
+      <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>362</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>637</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>639</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>300</v>
@@ -6152,23 +6263,26 @@
         <v>374</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>660</v>
+        <v>695</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6184,126 +6298,242 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>652</v>
+        <v>684</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>534</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>653</v>
+      <c r="K6" s="3" t="s">
+        <v>652</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>651</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>656</v>
+        <v>685</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>534</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H7" s="7">
         <v>1</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>653</v>
+      <c r="K7" s="3" t="s">
+        <v>652</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>651</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>657</v>
+        <v>693</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>534</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="P11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6434,13 +6664,13 @@
         <v>401</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>601</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6458,31 +6688,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C6" t="s">
         <v>550</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>551</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>552</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>553</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>554</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>555</v>
       </c>
-      <c r="G6" t="s">
-        <v>556</v>
-      </c>
-      <c r="H6" t="s">
-        <v>557</v>
-      </c>
       <c r="I6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified test data to include files in different index
</commit_message>
<xml_diff>
--- a/integration/10x.xlsx
+++ b/integration/10x.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/ait/repos/ingest-archiver/integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4955F8EA-F6E6-6941-A493-785BB8D22F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D397DE1-58D2-5049-B792-272FA5156113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="699">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -2128,6 +2128,15 @@
   </si>
   <si>
     <t>process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L002_R1_002.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L002_R2_002.fastq.gz</t>
+  </si>
+  <si>
+    <t>small_WSSS_THYst9384954_S1_L002_I1_002.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -4156,7 +4165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -6101,15 +6110,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="9" width="25.6640625" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
@@ -6534,6 +6543,123 @@
         <v>654</v>
       </c>
       <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="H14" s="7">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>654</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Remove user friendly column names
</commit_message>
<xml_diff>
--- a/integration/10x.xlsx
+++ b/integration/10x.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/ait/repos/ingest-archiver/integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D397DE1-58D2-5049-B792-272FA5156113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B052D5AA-57D5-0A49-8957-60D46F503667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="667">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -1107,84 +1107,18 @@
     <t xml:space="preserve"> For example: Should be one of: 'OK', 'control, 2-cell well', 'control, empty well', or 'low quality cell'.</t>
   </si>
   <si>
-    <t>FILE NAME (Required)</t>
-  </si>
-  <si>
-    <t>The filename of the file.</t>
-  </si>
-  <si>
-    <t>FILE FORMAT (Required)</t>
-  </si>
-  <si>
-    <t>The format of the file.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For example: fastq.gz</t>
-  </si>
-  <si>
-    <t>CHECKSUM</t>
-  </si>
-  <si>
-    <t>MD5 checksum of the file.</t>
-  </si>
-  <si>
     <t>sequence_file.file_core.file_name</t>
   </si>
   <si>
-    <t>READ INDEX (Required)</t>
-  </si>
-  <si>
-    <t>The sequencing read this file represents.</t>
-  </si>
-  <si>
-    <t>If a sequencing experiment is single-end, enter 'read1'. For example: Should be one of: read1, read2, index1, index2</t>
-  </si>
-  <si>
     <t>sequence_file.read_index</t>
   </si>
   <si>
-    <t>LANE INDEX</t>
-  </si>
-  <si>
-    <t>The lane that this file was sequenced from.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For example: 1</t>
-  </si>
-  <si>
     <t>sequence_file.lane_index</t>
   </si>
   <si>
-    <t>READ LENGTH</t>
-  </si>
-  <si>
-    <t>The length of a sequenced read in this file, in nucleotides.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For example: 51</t>
-  </si>
-  <si>
     <t>sequence_file.read_length</t>
   </si>
   <si>
-    <t>INSDC RUN ACCESSION</t>
-  </si>
-  <si>
-    <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession from the DDBJ, NCBI, or EMBL-EBI.</t>
-  </si>
-  <si>
-    <t>Accession must start with DRR, SRR, or ERR. For example: SRR0000000</t>
-  </si>
-  <si>
-    <t>LIBRARY PREPARATION ID</t>
-  </si>
-  <si>
-    <t>A unique ID for the library preparation.</t>
-  </si>
-  <si>
-    <t>Indicate which samples are from the same library preparation by providing a unique identifier for each library preparation. For example: tech_rep_group_001</t>
-  </si>
-  <si>
     <t>sequence_file.library_prep_id</t>
   </si>
   <si>
@@ -1938,15 +1872,6 @@
     <t>sequence_file.insdc_run_accessions</t>
   </si>
   <si>
-    <t>General description of the contents of the file.</t>
-  </si>
-  <si>
-    <t>An ontology term identifier in the form prefix:accession.</t>
-  </si>
-  <si>
-    <t>The preferred label for the ontology term referred to in the ontology field. This may differ from the user-supplied value in the text field.</t>
-  </si>
-  <si>
     <t>sequence_file.file_core.content_description.text</t>
   </si>
   <si>
@@ -1954,27 +1879,6 @@
   </si>
   <si>
     <t>sequence_file.file_core.content_description.ontology_label</t>
-  </si>
-  <si>
-    <t>For example: DNA sequence (raw); Sequence alignment</t>
-  </si>
-  <si>
-    <t>For example: DATA:3497; DATA:0863</t>
-  </si>
-  <si>
-    <t>CONTENT DESCRIPTION</t>
-  </si>
-  <si>
-    <t>CONTENT DESCRIPTION ONTOLOGY</t>
-  </si>
-  <si>
-    <t>CONTENT DESCRIPTION ONTOLOGY LABEL</t>
-  </si>
-  <si>
-    <t>SOURCE CELL SUSPENSION ID</t>
-  </si>
-  <si>
-    <t>PROCESS ID</t>
   </si>
   <si>
     <t>DNA sequence</t>
@@ -2635,7 +2539,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>648</v>
+        <v>616</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2644,7 +2548,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>647</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2661,16 +2565,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>584</v>
+        <v>562</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>585</v>
+        <v>563</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>586</v>
+        <v>564</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>587</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2687,13 +2591,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
       <c r="B6" t="s">
-        <v>682</v>
+        <v>650</v>
       </c>
       <c r="C6" t="s">
-        <v>683</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -2719,54 +2623,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>413</v>
+        <v>391</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>128</v>
@@ -2786,13 +2690,13 @@
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -2806,31 +2710,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>603</v>
+        <v>581</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>604</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2848,31 +2752,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>561</v>
+        <v>539</v>
       </c>
       <c r="B6" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
       <c r="C6" t="s">
-        <v>557</v>
+        <v>535</v>
       </c>
       <c r="D6" t="s">
-        <v>551</v>
+        <v>529</v>
       </c>
       <c r="E6" t="s">
-        <v>552</v>
+        <v>530</v>
       </c>
       <c r="F6" t="s">
-        <v>553</v>
+        <v>531</v>
       </c>
       <c r="G6" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="H6" t="s">
-        <v>558</v>
+        <v>536</v>
       </c>
       <c r="I6" t="s">
-        <v>559</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -2899,63 +2803,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>423</v>
+        <v>401</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>128</v>
@@ -2964,13 +2868,13 @@
         <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -2984,13 +2888,13 @@
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -3002,51 +2906,51 @@
         <v>82</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>419</v>
+        <v>397</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>621</v>
+        <v>599</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>622</v>
+        <v>600</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>623</v>
+        <v>601</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>624</v>
+        <v>602</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>625</v>
+        <v>603</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3067,34 +2971,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>562</v>
+        <v>540</v>
       </c>
       <c r="B6" t="s">
-        <v>563</v>
+        <v>541</v>
       </c>
       <c r="C6" t="s">
-        <v>564</v>
+        <v>542</v>
       </c>
       <c r="D6" t="s">
-        <v>551</v>
+        <v>529</v>
       </c>
       <c r="E6" t="s">
-        <v>552</v>
+        <v>530</v>
       </c>
       <c r="F6" t="s">
-        <v>553</v>
+        <v>531</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>566</v>
+        <v>544</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>567</v>
+        <v>545</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>568</v>
+        <v>546</v>
       </c>
       <c r="J6" t="s">
-        <v>565</v>
+        <v>543</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3243,94 +3147,94 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>436</v>
+        <v>414</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>437</v>
+        <v>415</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>438</v>
+        <v>416</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>439</v>
+        <v>417</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>440</v>
+        <v>418</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>441</v>
+        <v>419</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>442</v>
+        <v>420</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>443</v>
+        <v>421</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>593</v>
+        <v>571</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>592</v>
+        <v>570</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>591</v>
+        <v>569</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>663</v>
+        <v>631</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>664</v>
+        <v>632</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>665</v>
+        <v>633</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>666</v>
+        <v>634</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>668</v>
+        <v>636</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>669</v>
+        <v>637</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>670</v>
+        <v>638</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>671</v>
+        <v>639</v>
       </c>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3371,46 +3275,46 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>656</v>
+        <v>624</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>569</v>
+        <v>547</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>570</v>
+        <v>548</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>569</v>
+        <v>547</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>659</v>
+        <v>627</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>660</v>
+        <v>628</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>661</v>
+        <v>629</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>575</v>
+        <v>553</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>662</v>
+        <v>630</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -3423,20 +3327,20 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
-        <v>573</v>
+        <v>551</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>574</v>
+        <v>552</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>575</v>
+        <v>553</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>576</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="16" x14ac:dyDescent="0.2">
@@ -3484,69 +3388,69 @@
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>459</v>
+        <v>437</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>465</v>
+        <v>443</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>469</v>
+        <v>447</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>471</v>
+        <v>449</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>472</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>128</v>
@@ -3555,13 +3459,13 @@
         <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>462</v>
+        <v>440</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>466</v>
+        <v>444</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>470</v>
+        <v>448</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>128</v>
@@ -3581,13 +3485,13 @@
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -3599,10 +3503,10 @@
         <v>82</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>463</v>
+        <v>441</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>467</v>
+        <v>445</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>82</v>
@@ -3616,58 +3520,58 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>451</v>
+        <v>429</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>460</v>
+        <v>438</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>464</v>
+        <v>442</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>468</v>
+        <v>446</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>605</v>
+        <v>583</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>606</v>
+        <v>584</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>607</v>
+        <v>585</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>672</v>
+        <v>640</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>673</v>
+        <v>641</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>674</v>
+        <v>642</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>675</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3694,38 +3598,38 @@
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>676</v>
+        <v>644</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>677</v>
+        <v>645</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>678</v>
+        <v>646</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>679</v>
+        <v>647</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>678</v>
+        <v>646</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>487</v>
+        <v>465</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>680</v>
+        <v>648</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>681</v>
+        <v>649</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>680</v>
+        <v>648</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -3850,7 +3754,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -3874,7 +3778,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>614</v>
+        <v>592</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -3896,66 +3800,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="D6" t="s">
-        <v>480</v>
+        <v>458</v>
       </c>
       <c r="E6" t="s">
-        <v>481</v>
+        <v>459</v>
       </c>
       <c r="F6" t="s">
-        <v>483</v>
+        <v>461</v>
       </c>
       <c r="G6" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="H6" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="I6" t="s">
-        <v>488</v>
+        <v>466</v>
       </c>
       <c r="J6" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>474</v>
+        <v>452</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="C7" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="D7" t="s">
-        <v>479</v>
+        <v>457</v>
       </c>
       <c r="E7" t="s">
-        <v>482</v>
+        <v>460</v>
       </c>
       <c r="F7" t="s">
-        <v>484</v>
+        <v>462</v>
       </c>
       <c r="G7" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="H7" t="s">
-        <v>487</v>
+        <v>465</v>
       </c>
       <c r="I7" t="s">
-        <v>489</v>
+        <v>467</v>
       </c>
       <c r="J7" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -4035,7 +3939,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>612</v>
+        <v>590</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4044,7 +3948,7 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>613</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4058,19 +3962,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="B6" t="s">
-        <v>492</v>
+        <v>470</v>
       </c>
       <c r="C6" t="s">
-        <v>493</v>
+        <v>471</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -4135,7 +4039,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>583</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4147,13 +4051,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="B6" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="C6" t="s">
-        <v>497</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -4165,7 +4069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -4631,10 +4535,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>615</v>
+        <v>593</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>616</v>
+        <v>594</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -4795,115 +4699,115 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="B6" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="C6" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="F6" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="P6" t="s">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="Q6" t="s">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="R6" t="s">
-        <v>509</v>
+        <v>487</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>511</v>
+        <v>489</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="V6" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="W6" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
       <c r="X6" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="Y6" t="s">
-        <v>577</v>
+        <v>555</v>
       </c>
       <c r="Z6" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="AA6" t="s">
-        <v>577</v>
+        <v>555</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>515</v>
+        <v>493</v>
       </c>
       <c r="AE6" t="s">
-        <v>516</v>
+        <v>494</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="AH6" t="s">
-        <v>518</v>
+        <v>496</v>
       </c>
       <c r="AI6" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>520</v>
+        <v>498</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>519</v>
+        <v>497</v>
       </c>
       <c r="AM6" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -5284,10 +5188,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>618</v>
+        <v>596</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>617</v>
+        <v>595</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5308,13 +5212,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>594</v>
+        <v>572</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5332,7 +5236,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>597</v>
+        <v>575</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5344,7 +5248,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>598</v>
+        <v>576</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5374,7 +5278,7 @@
         <v>96</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5420,109 +5324,109 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>522</v>
+        <v>500</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>523</v>
+        <v>501</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="L6" t="s">
         <v>502</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="M6" t="s">
+        <v>503</v>
+      </c>
+      <c r="N6" t="s">
+        <v>502</v>
+      </c>
+      <c r="O6" t="s">
+        <v>557</v>
+      </c>
+      <c r="P6" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>557</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="U6" t="s">
+        <v>504</v>
+      </c>
+      <c r="V6" t="s">
+        <v>505</v>
+      </c>
+      <c r="W6" t="s">
         <v>506</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="X6" t="s">
         <v>507</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="L6" t="s">
-        <v>524</v>
-      </c>
-      <c r="M6" t="s">
-        <v>525</v>
-      </c>
-      <c r="N6" t="s">
-        <v>524</v>
-      </c>
-      <c r="O6" t="s">
-        <v>579</v>
-      </c>
-      <c r="P6" t="s">
-        <v>580</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>579</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="U6" t="s">
-        <v>526</v>
-      </c>
-      <c r="V6" t="s">
-        <v>527</v>
-      </c>
-      <c r="W6" t="s">
-        <v>528</v>
-      </c>
-      <c r="X6" t="s">
-        <v>529</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
       <c r="AA6" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>582</v>
+        <v>560</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>515</v>
+        <v>493</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>516</v>
+        <v>494</v>
       </c>
       <c r="AH6" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="AI6" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>548</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -5630,13 +5534,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>610</v>
+        <v>588</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>611</v>
+        <v>589</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>590</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -5825,10 +5729,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>619</v>
+        <v>597</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>620</v>
+        <v>598</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -5867,34 +5771,34 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>626</v>
+        <v>604</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>627</v>
+        <v>605</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>628</v>
+        <v>606</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>588</v>
+        <v>566</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>608</v>
+        <v>586</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>609</v>
+        <v>587</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>589</v>
+        <v>567</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5933,67 +5837,67 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>691</v>
+        <v>659</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="I6" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="J6" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="K6" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="L6" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
       <c r="M6" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
       <c r="P6" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="U6" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="V6" t="s">
-        <v>543</v>
+        <v>521</v>
       </c>
       <c r="W6" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6002,84 +5906,84 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>544</v>
+        <v>522</v>
       </c>
       <c r="AA6" t="s">
-        <v>581</v>
+        <v>559</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>561</v>
+        <v>539</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>562</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>692</v>
+        <v>660</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>690</v>
+        <v>658</v>
       </c>
       <c r="D7" s="3">
         <v>9606</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="N7" s="3">
         <v>98.7</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
       <c r="Q7" s="3">
         <v>10</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>543</v>
+        <v>521</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="X7" s="3">
         <v>1</v>
@@ -6088,19 +5992,19 @@
         <v>2217</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>544</v>
+        <v>522</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>581</v>
+        <v>559</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>561</v>
+        <v>539</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>562</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -6112,15 +6016,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="9" width="25.6640625" customWidth="1"/>
+    <col min="3" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="25.6640625" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
     <col min="11" max="11" width="26" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.33203125" style="3" customWidth="1"/>
@@ -6130,164 +6036,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>640</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>632</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="119" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>638</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>638</v>
-      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>629</v>
+        <v>607</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>635</v>
+        <v>610</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>636</v>
+        <v>611</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>300</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>631</v>
+        <v>609</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>695</v>
+        <v>663</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>655</v>
+        <v>623</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="P4" s="3"/>
     </row>
@@ -6311,354 +6147,354 @@
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>684</v>
+        <v>652</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
       <c r="H7" s="7">
         <v>1</v>
       </c>
       <c r="I7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>693</v>
+        <v>661</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
       </c>
       <c r="I8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>686</v>
+        <v>654</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>687</v>
+        <v>655</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
       <c r="H10" s="7">
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>694</v>
+        <v>662</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>696</v>
+        <v>664</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>697</v>
+        <v>665</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
       <c r="H13" s="7">
         <v>2</v>
       </c>
       <c r="I13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>698</v>
+        <v>666</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
       <c r="H14" s="7">
         <v>2</v>
       </c>
       <c r="I14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -6685,54 +6521,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>128</v>
@@ -6752,13 +6588,13 @@
         <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -6772,31 +6608,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>601</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6814,31 +6650,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>548</v>
+        <v>526</v>
       </c>
       <c r="B6" t="s">
-        <v>549</v>
+        <v>527</v>
       </c>
       <c r="C6" t="s">
-        <v>550</v>
+        <v>528</v>
       </c>
       <c r="D6" t="s">
-        <v>551</v>
+        <v>529</v>
       </c>
       <c r="E6" t="s">
-        <v>552</v>
+        <v>530</v>
       </c>
       <c r="F6" t="s">
-        <v>553</v>
+        <v>531</v>
       </c>
       <c r="G6" t="s">
-        <v>554</v>
+        <v>532</v>
       </c>
       <c r="H6" t="s">
-        <v>555</v>
+        <v>533</v>
       </c>
       <c r="I6" t="s">
-        <v>554</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>